<commit_message>
Sync data files - 2025-07-22 12:57:11 (       2 files updated)
</commit_message>
<xml_diff>
--- a/Data/Transactions/Sidra_transactions.xlsx
+++ b/Data/Transactions/Sidra_transactions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levan/Documents/MegaValuationer/Data/Transactions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A2058-EA7B-A04A-86F0-054DEB274055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CE78D6-AF7F-4742-8F7C-873D1775B242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{A799E9DF-2EC2-BB4D-96E3-8DA9F4319B01}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$2047</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4291,8 +4291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F700BF2-D90E-3645-8A35-E07DB41A9042}">
   <dimension ref="A1:N2052"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>